<commit_message>
Junit white box testing and code coverage tool
</commit_message>
<xml_diff>
--- a/Docs/Lab3/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab3/Lab03_WBT_TCs_Form.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{940DDD3B-2224-4FD7-80C6-54C863B8DFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AFB2AD-78B2-4A9D-9F29-9DED1C2F8609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" firstSheet="3" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="105">
   <si>
     <t>VVSS, Info Romana, 2021-2022</t>
   </si>
@@ -65,36 +65,9 @@
     <t>Student 2:</t>
   </si>
   <si>
-    <t>1. Evidenţa filmelor din colecţia personală</t>
-  </si>
-  <si>
     <t>Student 3:</t>
   </si>
   <si>
-    <t>Un cinefil doreşte să îşi dezvolte un program pentru gestionarea filmelor din colecţia personală. Programul va permite următoarele operaţii:</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>F02.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> cautarea filmelor care au un anumit regizor (sau parti din numele regizorului);</t>
-    </r>
-  </si>
-  <si>
     <t>F02. Filtrarea taskurilor dintr o anumita perioada</t>
   </si>
   <si>
@@ -182,27 +155,6 @@
     <t>1-2-3-4(T)-5-6(T)-7(7)-8-9(T)-10-11-4(F)-12-13</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">F02. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>cautarea filmelor care au un anumit regizor (sau parti din numele regizorului).</t>
-    </r>
-  </si>
-  <si>
     <t>TC No.</t>
   </si>
   <si>
@@ -227,21 +179,6 @@
     <t>Loop (lc)</t>
   </si>
   <si>
-    <t>F02_Cond01 &gt; 100</t>
-  </si>
-  <si>
-    <t>F02_Cond02 &lt; 20</t>
-  </si>
-  <si>
-    <t>F02_Cond03 == i</t>
-  </si>
-  <si>
-    <t>F02_Condnn &lt; n</t>
-  </si>
-  <si>
-    <t>F02_Pnn</t>
-  </si>
-  <si>
     <t>n-1</t>
   </si>
   <si>
@@ -261,12 +198,6 @@
   </si>
   <si>
     <t>F02_TC01</t>
-  </si>
-  <si>
-    <t>1, 2,4, 6, 7</t>
-  </si>
-  <si>
-    <t>F01_TC02</t>
   </si>
   <si>
     <t>WBT Implemented TCs</t>
@@ -502,12 +433,81 @@
   <si>
     <t>nu</t>
   </si>
+  <si>
+    <t>Carp Iulia-Maria</t>
+  </si>
+  <si>
+    <t>Campean Ariana-Deborah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afisarea task-rilor active planificate intr-o anumita perioada de timp, precizata ca data si ora de inceput si data si ora de sfarsit, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">campuri aflate pe ferastra principala a aplicatiei . Prin apasarea butonului “show” ,toate taskurile care se afla in intervalul inchis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">precizat de utilizator vor fi afisate in tabelul de pe aceeasi fereastra .La apasarea butonului “Reset”, filtrarea va fi anulata. </t>
+  </si>
+  <si>
+    <t>Daca campurile nu au fost completate corespunzator,va aparea pe ecran un mesaj de eroare cu continutul : “Trebuie completate toate campurile”</t>
+  </si>
+  <si>
+    <t>F02. afisarea task-urilor desfasurate intr-un interval dat</t>
+  </si>
+  <si>
+    <t>i&lt;tasks.size()</t>
+  </si>
+  <si>
+    <t>nextTime!=null</t>
+  </si>
+  <si>
+    <t>nextTime.before(end)</t>
+  </si>
+  <si>
+    <t>nextTime.equals(end)</t>
+  </si>
+  <si>
+    <t>F02_P04</t>
+  </si>
+  <si>
+    <t>empty list</t>
+  </si>
+  <si>
+    <t>list containing one task out of the interval</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>F02_TC03</t>
+  </si>
+  <si>
+    <t>F02_TC04</t>
+  </si>
+  <si>
+    <t>list containing goodTask</t>
+  </si>
+  <si>
+    <t>1-2-3-4-5-6(T/F)-7(T)-9(F)-11-4(T/F)-12-13</t>
+  </si>
+  <si>
+    <t>1-2-3-4(T)-5-6(T)-7(F)-9(F)-11-4(F)-12-13</t>
+  </si>
+  <si>
+    <t>lista contains  Task badTask = new Task("Task1", new Date(start));
+        Task goodTask = new Task("Task1", new Date(start), new Date(end), 1);   start = 1;
+end = System.currentTimeMillis();</t>
+  </si>
+  <si>
+    <t>list contains     Task goodTask = new Task("Task1", new Date(start), new Date(start + 86400000), 86400000);       start = 1;
+end = System.currentTimeMillis();</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -619,13 +619,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="9"/>
@@ -638,6 +631,19 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1180,7 +1186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1228,12 +1234,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1270,9 +1270,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1285,194 +1284,204 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1917,29 +1926,29 @@
   <dimension ref="B1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="19.7109375" customWidth="1"/>
+    <col min="15" max="15" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="2" spans="2:16">
-      <c r="B2" s="41" t="s">
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="41"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B2" s="38" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:16">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1949,88 +1958,99 @@
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
     </row>
-    <row r="5" spans="2:16">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="37" t="s">
+      <c r="N5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-    </row>
-    <row r="6" spans="2:16">
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29" t="s">
+      <c r="N6" s="27"/>
+      <c r="O6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="29" t="s">
+      <c r="P6" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:16">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="N7" s="29" t="s">
+      <c r="N7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-    </row>
-    <row r="8" spans="2:16">
+      <c r="O7" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="P7" s="27">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="N8" s="29" t="s">
+      <c r="N8" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-    </row>
-    <row r="9" spans="2:16">
+      <c r="O8" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="P8" s="27">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="N9" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-    </row>
-    <row r="10" spans="2:16">
+      <c r="N9" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="2:16">
-      <c r="B11" s="39" t="s">
-        <v>14</v>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="106" t="s">
+        <v>87</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
     </row>
   </sheetData>
@@ -2049,371 +2069,380 @@
   </sheetPr>
   <dimension ref="B1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView topLeftCell="I10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18:T18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" customWidth="1"/>
+    <col min="20" max="20" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="44"/>
-    </row>
-    <row r="3" spans="2:20">
-      <c r="B3" s="48" t="s">
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="41"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B3" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="45"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B6" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="I6" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="Q6" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="50"/>
-    </row>
-    <row r="6" spans="2:20">
-      <c r="B6" s="42" t="s">
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B8" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="I6" s="42" t="s">
+      <c r="C8" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="Q6" s="42" t="s">
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="I8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="R6" s="43"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="43"/>
-    </row>
-    <row r="8" spans="2:20">
-      <c r="B8" s="34" t="s">
+      <c r="Q8" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="I8" s="12" t="s">
+      <c r="R8" s="56"/>
+      <c r="S8" s="56"/>
+      <c r="T8" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B9" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="Q8" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="R8" s="47"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="2:20">
-      <c r="B9" s="37" t="s">
-        <v>24</v>
-      </c>
       <c r="C9" s="46" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D9" s="46"/>
       <c r="E9" s="46"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="I9" s="40"/>
-      <c r="Q9" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="R9" s="47"/>
-      <c r="S9" s="47"/>
-      <c r="T9" s="36" t="s">
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="I9" s="37"/>
+      <c r="Q9" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" s="56"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B10" s="35" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="2:20">
-      <c r="B10" s="37" t="s">
-        <v>26</v>
-      </c>
       <c r="C10" s="46" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="46"/>
       <c r="E10" s="46"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="I10" s="51" t="s">
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="I10" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="49"/>
+      <c r="Q10" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="R10" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="S10" s="56"/>
+      <c r="T10" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B11" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="53"/>
-      <c r="Q10" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="S10" s="47"/>
-      <c r="T10" s="36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20">
-      <c r="B11" s="37" t="s">
-        <v>30</v>
-      </c>
       <c r="C11" s="46" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="46"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="56"/>
-    </row>
-    <row r="12" spans="2:20">
-      <c r="B12" s="37" t="s">
-        <v>31</v>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="52"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B12" s="35" t="s">
+        <v>28</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D12" s="46"/>
       <c r="E12" s="46"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="56"/>
-    </row>
-    <row r="13" spans="2:20">
-      <c r="B13" s="37" t="s">
-        <v>32</v>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="52"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B13" s="35" t="s">
+        <v>29</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D13" s="46"/>
       <c r="E13" s="46"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55"/>
-      <c r="M13" s="55"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="56"/>
-      <c r="Q13" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="R13" s="43"/>
-      <c r="S13" s="43"/>
-      <c r="T13" s="43"/>
-    </row>
-    <row r="14" spans="2:20">
-      <c r="B14" s="37" t="s">
-        <v>31</v>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="52"/>
+      <c r="Q13" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B14" s="35" t="s">
+        <v>28</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D14" s="46"/>
       <c r="E14" s="46"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="55"/>
-      <c r="N14" s="55"/>
-      <c r="O14" s="56"/>
-    </row>
-    <row r="15" spans="2:20">
-      <c r="I15" s="54"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="55"/>
-      <c r="M15" s="55"/>
-      <c r="N15" s="55"/>
-      <c r="O15" s="56"/>
-      <c r="Q15" s="34" t="s">
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="52"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="I15" s="50"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="52"/>
+      <c r="Q15" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="R15" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="I16" s="50"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="52"/>
+      <c r="Q16" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="R16" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="R15" s="60" t="s">
+      <c r="S16" s="42"/>
+      <c r="T16" s="42"/>
+    </row>
+    <row r="17" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I17" s="50"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="52"/>
+      <c r="Q17" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="S15" s="60"/>
-      <c r="T15" s="60"/>
-    </row>
-    <row r="16" spans="2:20">
-      <c r="I16" s="54"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="55"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="56"/>
-      <c r="Q16" s="37" t="s">
+      <c r="R17" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="R16" s="45" t="s">
+      <c r="S17" s="42"/>
+      <c r="T17" s="42"/>
+    </row>
+    <row r="18" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I18" s="50"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="52"/>
+      <c r="Q18" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-    </row>
-    <row r="17" spans="9:20">
-      <c r="I17" s="54"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="55"/>
-      <c r="M17" s="55"/>
-      <c r="N17" s="55"/>
-      <c r="O17" s="56"/>
-      <c r="Q17" s="37" t="s">
+      <c r="R18" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="R17" s="45" t="s">
+      <c r="S18" s="42"/>
+      <c r="T18" s="42"/>
+    </row>
+    <row r="19" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I19" s="50"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="52"/>
+      <c r="Q19" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="S17" s="45"/>
-      <c r="T17" s="45"/>
-    </row>
-    <row r="18" spans="9:20">
-      <c r="I18" s="54"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="55"/>
-      <c r="M18" s="55"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="56"/>
-      <c r="Q18" s="37" t="s">
+      <c r="R19" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="R18" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-    </row>
-    <row r="19" spans="9:20">
-      <c r="I19" s="54"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="55"/>
-      <c r="L19" s="55"/>
-      <c r="M19" s="55"/>
-      <c r="N19" s="55"/>
-      <c r="O19" s="56"/>
-      <c r="Q19" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="R19" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="S19" s="45"/>
-      <c r="T19" s="45"/>
-    </row>
-    <row r="20" spans="9:20">
-      <c r="I20" s="54"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="55"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="55"/>
-      <c r="O20" s="56"/>
-      <c r="Q20" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="R20" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="S20" s="45"/>
-      <c r="T20" s="45"/>
-    </row>
-    <row r="21" spans="9:20">
-      <c r="I21" s="54"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="56"/>
-      <c r="Q21" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="R21" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="S21" s="45"/>
-      <c r="T21" s="45"/>
-    </row>
-    <row r="22" spans="9:20">
-      <c r="I22" s="54"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="55"/>
-      <c r="M22" s="55"/>
-      <c r="N22" s="55"/>
-      <c r="O22" s="56"/>
-    </row>
-    <row r="23" spans="9:20">
-      <c r="I23" s="54"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="55"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="55"/>
-      <c r="O23" s="56"/>
-    </row>
-    <row r="24" spans="9:20">
-      <c r="I24" s="57"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="58"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="58"/>
-      <c r="N24" s="58"/>
-      <c r="O24" s="59"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="42"/>
+    </row>
+    <row r="20" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I20" s="50"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="52"/>
+      <c r="Q20" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="R20" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="S20" s="42"/>
+      <c r="T20" s="42"/>
+    </row>
+    <row r="21" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I21" s="50"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="52"/>
+      <c r="Q21" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="R21" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="S21" s="42"/>
+      <c r="T21" s="42"/>
+    </row>
+    <row r="22" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I22" s="50"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="52"/>
+    </row>
+    <row r="23" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I23" s="50"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="52"/>
+    </row>
+    <row r="24" spans="9:20" x14ac:dyDescent="0.3">
+      <c r="I24" s="53"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="R21:T21"/>
@@ -2430,14 +2459,6 @@
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2452,258 +2473,254 @@
   </sheetPr>
   <dimension ref="B1:AB16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" customWidth="1"/>
-    <col min="12" max="12" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.21875" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" customWidth="1"/>
+    <col min="12" max="12" width="6.44140625" customWidth="1"/>
     <col min="13" max="13" width="5" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" customWidth="1"/>
-    <col min="16" max="17" width="8.85546875" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" customWidth="1"/>
-    <col min="22" max="24" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" customWidth="1"/>
+    <col min="16" max="17" width="8.88671875" customWidth="1"/>
+    <col min="21" max="21" width="9.109375" customWidth="1"/>
+    <col min="22" max="24" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28">
+    <row r="1" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="3" spans="2:28">
-      <c r="B3" s="48" t="s">
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="41"/>
+    </row>
+    <row r="3" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B3" s="107" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
+    </row>
+    <row r="5" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B5" s="11"/>
+    </row>
+    <row r="6" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
-    </row>
-    <row r="5" spans="2:28">
-      <c r="B5" s="11"/>
-    </row>
-    <row r="6" spans="2:28" ht="15.75">
-      <c r="B6" s="65" t="s">
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="58"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="58"/>
+      <c r="W6" s="58"/>
+      <c r="X6" s="58"/>
+      <c r="Y6" s="58"/>
+      <c r="Z6" s="58"/>
+      <c r="AA6" s="58"/>
+      <c r="AB6" s="58"/>
+    </row>
+    <row r="7" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="F7" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="66" t="s">
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="Q7" s="62"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="62"/>
+      <c r="T7" s="62"/>
+      <c r="U7" s="62"/>
+      <c r="V7" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="65"/>
-      <c r="S6" s="65"/>
-      <c r="T6" s="65"/>
-      <c r="U6" s="65"/>
-      <c r="V6" s="65"/>
-      <c r="W6" s="65"/>
-      <c r="X6" s="65"/>
-      <c r="Y6" s="65"/>
-      <c r="Z6" s="65"/>
-      <c r="AA6" s="65"/>
-      <c r="AB6" s="65"/>
-    </row>
-    <row r="7" spans="2:28" ht="15.75">
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="61" t="s">
+      <c r="W7" s="61"/>
+      <c r="X7" s="61"/>
+      <c r="Y7" s="61"/>
+      <c r="Z7" s="61"/>
+      <c r="AA7" s="61"/>
+      <c r="AB7" s="61"/>
+    </row>
+    <row r="8" spans="2:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="58"/>
+      <c r="C8" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="66"/>
+      <c r="F8" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="65"/>
+      <c r="N8" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="O8" s="65"/>
+      <c r="P8" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="R8" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="S8" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="T8" s="62"/>
+      <c r="U8" s="62"/>
+      <c r="V8" s="61">
+        <v>0</v>
+      </c>
+      <c r="W8" s="61">
+        <v>1</v>
+      </c>
+      <c r="X8" s="61">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="62" t="s">
+      <c r="Z8" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="63" t="s">
+      <c r="AA8" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="Q7" s="63"/>
-      <c r="R7" s="63"/>
-      <c r="S7" s="63"/>
-      <c r="T7" s="63"/>
-      <c r="U7" s="63"/>
-      <c r="V7" s="64" t="s">
+      <c r="AB8" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="W7" s="64"/>
-      <c r="X7" s="64"/>
-      <c r="Y7" s="64"/>
-      <c r="Z7" s="64"/>
-      <c r="AA7" s="64"/>
-      <c r="AB7" s="64"/>
-    </row>
-    <row r="8" spans="2:28" ht="15.6" customHeight="1">
-      <c r="B8" s="65"/>
-      <c r="C8" s="68" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="68" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="61"/>
-      <c r="F8" s="62" t="s">
+    </row>
+    <row r="9" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="58"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62" t="s">
+      <c r="G9" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62" t="s">
+      <c r="H9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="62"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="61"/>
+      <c r="W9" s="61"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="61"/>
+      <c r="Z9" s="61"/>
+      <c r="AA9" s="61"/>
+      <c r="AB9" s="61"/>
+    </row>
+    <row r="10" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="O8" s="62"/>
-      <c r="P8" s="63" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q8" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="R8" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="S8" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="T8" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="U8" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="V8" s="64">
-        <v>0</v>
-      </c>
-      <c r="W8" s="64">
-        <v>1</v>
-      </c>
-      <c r="X8" s="64">
-        <v>2</v>
-      </c>
-      <c r="Y8" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z8" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA8" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB8" s="64" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="2:28" ht="15.75">
-      <c r="B9" s="65"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="N9" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="O9" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="63"/>
-      <c r="S9" s="63"/>
-      <c r="T9" s="63"/>
-      <c r="U9" s="63"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="64"/>
-      <c r="X9" s="64"/>
-      <c r="Y9" s="64"/>
-      <c r="Z9" s="64"/>
-      <c r="AA9" s="64"/>
-      <c r="AB9" s="64"/>
-    </row>
-    <row r="10" spans="2:28" ht="15.75">
-      <c r="B10" s="14" t="s">
-        <v>64</v>
-      </c>
       <c r="C10" s="14" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -2715,13 +2732,17 @@
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
-      <c r="P10" s="18"/>
+      <c r="P10" s="18" t="s">
+        <v>97</v>
+      </c>
       <c r="Q10" s="18"/>
       <c r="R10" s="18"/>
       <c r="S10" s="18"/>
       <c r="T10" s="18"/>
       <c r="U10" s="18"/>
-      <c r="V10" s="19"/>
+      <c r="V10" s="19" t="s">
+        <v>97</v>
+      </c>
       <c r="W10" s="19"/>
       <c r="X10" s="19"/>
       <c r="Y10" s="19"/>
@@ -2729,17 +2750,19 @@
       <c r="AA10" s="19"/>
       <c r="AB10" s="19"/>
     </row>
-    <row r="11" spans="2:28" ht="15.75">
+    <row r="11" spans="2:28" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="16"/>
+        <v>95</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>102</v>
+      </c>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
@@ -2752,35 +2775,57 @@
       <c r="O11" s="17"/>
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
+      <c r="R11" s="18" t="s">
+        <v>97</v>
+      </c>
       <c r="S11" s="18"/>
       <c r="T11" s="18"/>
       <c r="U11" s="18"/>
       <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
+      <c r="W11" s="19" t="s">
+        <v>97</v>
+      </c>
       <c r="X11" s="19"/>
       <c r="Y11" s="19"/>
       <c r="Z11" s="19"/>
       <c r="AA11" s="19"/>
       <c r="AB11" s="19"/>
     </row>
-    <row r="12" spans="2:28" ht="15.75">
+    <row r="12" spans="2:28" ht="202.8" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
+        <v>98</v>
+      </c>
+      <c r="C12" s="108" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="109" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
+      <c r="O12" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="P12" s="18"/>
       <c r="Q12" s="18"/>
       <c r="R12" s="18"/>
@@ -2789,28 +2834,42 @@
       <c r="U12" s="18"/>
       <c r="V12" s="19"/>
       <c r="W12" s="19"/>
-      <c r="X12" s="19"/>
+      <c r="X12" s="19" t="s">
+        <v>97</v>
+      </c>
       <c r="Y12" s="19"/>
       <c r="Z12" s="19"/>
       <c r="AA12" s="19"/>
       <c r="AB12" s="19"/>
     </row>
-    <row r="13" spans="2:28" ht="15.75">
+    <row r="13" spans="2:28" ht="171.6" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="14"/>
+        <v>99</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>104</v>
+      </c>
       <c r="D13" s="15"/>
       <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
+      <c r="F13" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
+      <c r="K13" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="L13" s="17"/>
       <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
+      <c r="N13" s="17" t="s">
+        <v>53</v>
+      </c>
       <c r="O13" s="17"/>
       <c r="P13" s="18"/>
       <c r="Q13" s="18"/>
@@ -2826,10 +2885,8 @@
       <c r="AA13" s="19"/>
       <c r="AB13" s="19"/>
     </row>
-    <row r="14" spans="2:28" ht="15.75">
-      <c r="B14" s="14" t="s">
-        <v>23</v>
-      </c>
+    <row r="14" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="15"/>
       <c r="E14" s="16"/>
@@ -2857,10 +2914,8 @@
       <c r="AA14" s="19"/>
       <c r="AB14" s="19"/>
     </row>
-    <row r="15" spans="2:28" ht="15.75">
-      <c r="B15" s="14" t="s">
-        <v>23</v>
-      </c>
+    <row r="15" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="15"/>
       <c r="E15" s="16"/>
@@ -2888,11 +2943,25 @@
       <c r="AA15" s="19"/>
       <c r="AB15" s="19"/>
     </row>
-    <row r="16" spans="2:28" ht="15.75">
-      <c r="B16" s="22"/>
+    <row r="16" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:O7"/>
+    <mergeCell ref="P7:U7"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="V7:AB7"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
@@ -2909,20 +2978,6 @@
     <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:O7"/>
-    <mergeCell ref="P7:U7"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="V7:AB7"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2940,253 +2995,253 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="44"/>
-    </row>
-    <row r="3" spans="2:14">
-      <c r="B3" s="95" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-    </row>
-    <row r="4" spans="2:14">
-      <c r="B4" s="96" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="102" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="84" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="84" t="s">
-        <v>72</v>
-      </c>
-      <c r="L4" s="85"/>
-    </row>
-    <row r="5" spans="2:14" ht="15.75" thickBot="1">
-      <c r="B5" s="97"/>
-      <c r="C5" s="101"/>
-      <c r="D5" s="103"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="41"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="84" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="75" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" s="76"/>
+    </row>
+    <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="74"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="85"/>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="86" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="87"/>
+        <v>20</v>
+      </c>
+      <c r="I5" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="78"/>
       <c r="K5" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" ht="15.75" thickTop="1">
-      <c r="B6" s="23">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="21">
         <v>9</v>
       </c>
-      <c r="C6" s="98" t="s">
-        <v>75</v>
+      <c r="C6" s="79" t="s">
+        <v>64</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="82" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="83"/>
-      <c r="K6" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14">
-      <c r="B7" s="23">
+        <v>55</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="92" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="93"/>
+      <c r="K6" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="21">
         <v>10</v>
       </c>
-      <c r="C7" s="98"/>
+      <c r="C7" s="79"/>
       <c r="D7" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="23">
+        <v>65</v>
+      </c>
+      <c r="E7" s="21">
         <v>5</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="21">
         <v>6</v>
       </c>
-      <c r="G7" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="84" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="85"/>
-      <c r="K7" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14">
-      <c r="B8" s="23">
+      <c r="G7" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="76"/>
+      <c r="K7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="21">
         <v>11</v>
       </c>
-      <c r="C8" s="98"/>
+      <c r="C8" s="79"/>
       <c r="D8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="84" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="85"/>
-      <c r="K8" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14">
-      <c r="B9" s="23">
+        <v>20</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="76"/>
+      <c r="K8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="21">
         <v>12</v>
       </c>
-      <c r="C9" s="98"/>
+      <c r="C9" s="79"/>
       <c r="D9" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="84" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="85"/>
-      <c r="K9" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="15.75" thickBot="1">
+        <v>20</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="76"/>
+      <c r="K9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>13</v>
       </c>
-      <c r="C10" s="99"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="86" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="87"/>
+        <v>20</v>
+      </c>
+      <c r="I10" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="78"/>
       <c r="K10" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" ht="15.75" thickTop="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -3199,131 +3254,149 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="2:14" ht="15.75" thickBot="1">
+    <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="23"/>
+    </row>
+    <row r="13" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="70"/>
+      <c r="H13" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="71"/>
+      <c r="M13" s="100" t="s">
+        <v>70</v>
+      </c>
+      <c r="N13" s="101"/>
+    </row>
+    <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="99" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="90" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="90" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="103" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="87" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="86" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="K12" s="25"/>
-    </row>
-    <row r="13" spans="2:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B13" s="104" t="s">
+      <c r="I14" s="90" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="90" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" s="94" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="106" t="s">
+      <c r="L14" s="96" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="107"/>
-      <c r="H13" s="104" t="s">
+      <c r="M14" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="I13" s="105"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="105"/>
-      <c r="L13" s="108"/>
-      <c r="M13" s="93" t="s">
+      <c r="N14" s="82" t="s">
         <v>81</v>
       </c>
-      <c r="N13" s="94"/>
-    </row>
-    <row r="14" spans="2:14" ht="15.75" thickTop="1">
-      <c r="B14" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" s="72" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" s="74" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" s="76" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" s="78" t="s">
-        <v>87</v>
-      </c>
-      <c r="H14" s="80" t="s">
-        <v>88</v>
-      </c>
-      <c r="I14" s="72" t="s">
-        <v>82</v>
-      </c>
-      <c r="J14" s="72" t="s">
-        <v>83</v>
-      </c>
-      <c r="K14" s="88" t="s">
-        <v>89</v>
-      </c>
-      <c r="L14" s="90" t="s">
-        <v>90</v>
-      </c>
-      <c r="M14" s="92" t="s">
-        <v>91</v>
-      </c>
-      <c r="N14" s="79" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14">
-      <c r="B15" s="71"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="73"/>
-      <c r="J15" s="73"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="91"/>
-      <c r="M15" s="70"/>
-      <c r="N15" s="76"/>
-    </row>
-    <row r="16" spans="2:14">
-      <c r="B16" s="29">
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="102"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="91"/>
+      <c r="K15" s="95"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="99"/>
+      <c r="N15" s="87"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="27">
         <f>SUM(C16:D16)</f>
         <v>0</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="24">
         <v>0</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="24">
         <v>0</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="26"/>
       <c r="G16" s="8" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="I16" s="29">
+        <v>82</v>
+      </c>
+      <c r="I16" s="27">
         <f>SUM(J16:K16)</f>
         <v>0</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="24">
         <v>0</v>
       </c>
-      <c r="K16" s="30">
+      <c r="K16" s="28">
         <v>0</v>
       </c>
-      <c r="L16" s="31"/>
+      <c r="L16" s="29"/>
       <c r="M16" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="N16" s="32">
+        <v>82</v>
+      </c>
+      <c r="N16" s="30">
         <f>C16</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="M13:N13"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:L13"/>
@@ -3337,24 +3410,6 @@
     <mergeCell ref="E4:J4"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3362,6 +3417,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003CE88883EE47F4428D9429E199926803" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f58aede59a59902c28a1e06604e86509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cb151dce-bb4e-4b45-9888-deda11e2455e" xmlns:ns3="851ad6cb-772e-4066-aadb-684825ca80fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66be19071027bf40cc935f24f7a086f4" ns2:_="" ns3:_="">
     <xsd:import namespace="cb151dce-bb4e-4b45-9888-deda11e2455e"/>
@@ -3550,19 +3614,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0310686C-5FB0-45DC-A155-16FD14CB70E3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD927A50-C247-4539-9D6B-11DFFC9ACCD7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD927A50-C247-4539-9D6B-11DFFC9ACCD7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0310686C-5FB0-45DC-A155-16FD14CB70E3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cb151dce-bb4e-4b45-9888-deda11e2455e"/>
+    <ds:schemaRef ds:uri="851ad6cb-772e-4066-aadb-684825ca80fc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Finished the XML file
</commit_message>
<xml_diff>
--- a/Docs/Lab3/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab3/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AFB2AD-78B2-4A9D-9F29-9DED1C2F8609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F43635-D7D5-4CA2-B379-EF3C4BF35AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="117">
   <si>
     <t>VVSS, Info Romana, 2021-2022</t>
   </si>
@@ -501,6 +501,42 @@
   <si>
     <t>list contains     Task goodTask = new Task("Task1", new Date(start), new Date(start + 86400000), 86400000);       start = 1;
 end = System.currentTimeMillis();</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>no data is inserted</t>
+  </si>
+  <si>
+    <t>Task1</t>
+  </si>
+  <si>
+    <t>Date(1)</t>
+  </si>
+  <si>
+    <t>none/cureent date</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>list contains just the good task</t>
+  </si>
+  <si>
+    <t>Date(86400001)</t>
+  </si>
+  <si>
+    <t>list contains the task</t>
   </si>
 </sst>
 </file>
@@ -1246,11 +1282,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1272,6 +1306,13 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1284,6 +1325,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1293,9 +1340,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1323,12 +1367,24 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1338,23 +1394,86 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1380,18 +1499,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1401,9 +1508,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1413,76 +1517,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1936,15 +1972,15 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="36" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1962,21 +1998,21 @@
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="35" t="s">
+      <c r="N5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27" t="s">
+      <c r="N6" s="26"/>
+      <c r="O6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="P6" s="27" t="s">
+      <c r="P6" s="26" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1985,13 +2021,13 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="N7" s="27" t="s">
+      <c r="N7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="27" t="s">
+      <c r="O7" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="P7" s="27">
+      <c r="P7" s="26">
         <v>232</v>
       </c>
     </row>
@@ -2000,13 +2036,13 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="N8" s="27" t="s">
+      <c r="N8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="27" t="s">
+      <c r="O8" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="P8" s="27">
+      <c r="P8" s="26">
         <v>232</v>
       </c>
     </row>
@@ -2017,11 +2053,11 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="N9" s="27" t="s">
+      <c r="N9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -2032,7 +2068,7 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="106" t="s">
+      <c r="B11" s="37" t="s">
         <v>87</v>
       </c>
       <c r="C11" s="1"/>
@@ -2069,7 +2105,7 @@
   </sheetPr>
   <dimension ref="B1:T24"/>
   <sheetViews>
-    <sheetView topLeftCell="I10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="I13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="R18" sqref="R18:T18"/>
     </sheetView>
   </sheetViews>
@@ -2082,367 +2118,359 @@
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="45"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="48"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="I6" s="39" t="s">
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="I6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="Q6" s="39" t="s">
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="Q6" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="R6" s="40"/>
-      <c r="S6" s="40"/>
-      <c r="T6" s="40"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
       <c r="I8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="Q8" s="56" t="s">
+      <c r="Q8" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="R8" s="56"/>
-      <c r="S8" s="56"/>
-      <c r="T8" s="34" t="s">
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="32" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="I9" s="37"/>
-      <c r="Q9" s="56" t="s">
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="I9" s="35"/>
+      <c r="Q9" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="R9" s="56"/>
-      <c r="S9" s="56"/>
-      <c r="T9" s="34" t="s">
+      <c r="R9" s="45"/>
+      <c r="S9" s="45"/>
+      <c r="T9" s="32" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="I10" s="47" t="s">
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="I10" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="49"/>
-      <c r="Q10" s="56" t="s">
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="51"/>
+      <c r="Q10" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="R10" s="56" t="s">
+      <c r="R10" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="S10" s="56"/>
-      <c r="T10" s="34" t="s">
+      <c r="S10" s="45"/>
+      <c r="T10" s="32" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="52"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="54"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="52"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="53"/>
+      <c r="O12" s="54"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="51"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="52"/>
-      <c r="Q13" s="39" t="s">
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="54"/>
+      <c r="Q13" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="R13" s="40"/>
-      <c r="S13" s="40"/>
-      <c r="T13" s="40"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="51"/>
-      <c r="O14" s="52"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="54"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="I15" s="50"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="52"/>
-      <c r="Q15" s="32" t="s">
+      <c r="I15" s="52"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="54"/>
+      <c r="Q15" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="R15" s="57" t="s">
+      <c r="R15" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="S15" s="57"/>
-      <c r="T15" s="57"/>
+      <c r="S15" s="58"/>
+      <c r="T15" s="58"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="I16" s="50"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="52"/>
-      <c r="Q16" s="35" t="s">
+      <c r="I16" s="52"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="54"/>
+      <c r="Q16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="R16" s="42" t="s">
+      <c r="R16" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="S16" s="42"/>
-      <c r="T16" s="42"/>
+      <c r="S16" s="43"/>
+      <c r="T16" s="43"/>
     </row>
     <row r="17" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I17" s="50"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="52"/>
-      <c r="Q17" s="35" t="s">
+      <c r="I17" s="52"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="54"/>
+      <c r="Q17" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="R17" s="42" t="s">
+      <c r="R17" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="S17" s="42"/>
-      <c r="T17" s="42"/>
+      <c r="S17" s="43"/>
+      <c r="T17" s="43"/>
     </row>
     <row r="18" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I18" s="50"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="52"/>
-      <c r="Q18" s="35" t="s">
+      <c r="I18" s="52"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="53"/>
+      <c r="O18" s="54"/>
+      <c r="Q18" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="R18" s="42" t="s">
+      <c r="R18" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="S18" s="42"/>
-      <c r="T18" s="42"/>
+      <c r="S18" s="43"/>
+      <c r="T18" s="43"/>
     </row>
     <row r="19" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I19" s="50"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="52"/>
-      <c r="Q19" s="35" t="s">
+      <c r="I19" s="52"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="53"/>
+      <c r="O19" s="54"/>
+      <c r="Q19" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="R19" s="42" t="s">
+      <c r="R19" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="S19" s="42"/>
-      <c r="T19" s="42"/>
+      <c r="S19" s="43"/>
+      <c r="T19" s="43"/>
     </row>
     <row r="20" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I20" s="50"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="52"/>
-      <c r="Q20" s="35" t="s">
+      <c r="I20" s="52"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
+      <c r="O20" s="54"/>
+      <c r="Q20" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="R20" s="42" t="s">
+      <c r="R20" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="S20" s="42"/>
-      <c r="T20" s="42"/>
+      <c r="S20" s="43"/>
+      <c r="T20" s="43"/>
     </row>
     <row r="21" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I21" s="50"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="52"/>
-      <c r="Q21" s="35" t="s">
+      <c r="I21" s="52"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
+      <c r="N21" s="53"/>
+      <c r="O21" s="54"/>
+      <c r="Q21" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="R21" s="42" t="s">
+      <c r="R21" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="S21" s="42"/>
-      <c r="T21" s="42"/>
+      <c r="S21" s="43"/>
+      <c r="T21" s="43"/>
     </row>
     <row r="22" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I22" s="50"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="54"/>
     </row>
     <row r="23" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I23" s="50"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="54"/>
     </row>
     <row r="24" spans="9:20" x14ac:dyDescent="0.3">
-      <c r="I24" s="53"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54"/>
-      <c r="O24" s="55"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="R21:T21"/>
@@ -2459,6 +2487,14 @@
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R18:T18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2473,8 +2509,8 @@
   </sheetPr>
   <dimension ref="B1:AB16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2502,169 +2538,169 @@
   <sheetData>
     <row r="1" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="45"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="48"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B5" s="11"/>
     </row>
     <row r="6" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="58" t="s">
+      <c r="E6" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="58"/>
-      <c r="X6" s="58"/>
-      <c r="Y6" s="58"/>
-      <c r="Z6" s="58"/>
-      <c r="AA6" s="58"/>
-      <c r="AB6" s="58"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="64"/>
+      <c r="Q6" s="64"/>
+      <c r="R6" s="64"/>
+      <c r="S6" s="64"/>
+      <c r="T6" s="64"/>
+      <c r="U6" s="64"/>
+      <c r="V6" s="64"/>
+      <c r="W6" s="64"/>
+      <c r="X6" s="64"/>
+      <c r="Y6" s="64"/>
+      <c r="Z6" s="64"/>
+      <c r="AA6" s="64"/>
+      <c r="AB6" s="64"/>
     </row>
     <row r="7" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="66" t="s">
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="65" t="s">
+      <c r="F7" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
-      <c r="O7" s="65"/>
-      <c r="P7" s="62" t="s">
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="62"/>
-      <c r="S7" s="62"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="62"/>
-      <c r="V7" s="61" t="s">
+      <c r="Q7" s="61"/>
+      <c r="R7" s="61"/>
+      <c r="S7" s="61"/>
+      <c r="T7" s="61"/>
+      <c r="U7" s="61"/>
+      <c r="V7" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="W7" s="61"/>
-      <c r="X7" s="61"/>
-      <c r="Y7" s="61"/>
-      <c r="Z7" s="61"/>
-      <c r="AA7" s="61"/>
-      <c r="AB7" s="61"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="62"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="62"/>
+      <c r="AA7" s="62"/>
+      <c r="AB7" s="62"/>
     </row>
     <row r="8" spans="2:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="58"/>
-      <c r="C8" s="63" t="s">
+      <c r="B8" s="64"/>
+      <c r="C8" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="66"/>
-      <c r="F8" s="65" t="s">
+      <c r="E8" s="59"/>
+      <c r="F8" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65" t="s">
+      <c r="G8" s="60"/>
+      <c r="H8" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="I8" s="65"/>
-      <c r="J8" s="65" t="s">
+      <c r="I8" s="60"/>
+      <c r="J8" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="K8" s="65"/>
-      <c r="L8" s="65" t="s">
+      <c r="K8" s="60"/>
+      <c r="L8" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="65"/>
-      <c r="N8" s="65" t="s">
+      <c r="M8" s="60"/>
+      <c r="N8" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="O8" s="65"/>
-      <c r="P8" s="62" t="s">
+      <c r="O8" s="60"/>
+      <c r="P8" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="Q8" s="62" t="s">
+      <c r="Q8" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="R8" s="62" t="s">
+      <c r="R8" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="S8" s="62" t="s">
+      <c r="S8" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="T8" s="62"/>
-      <c r="U8" s="62"/>
-      <c r="V8" s="61">
+      <c r="T8" s="61"/>
+      <c r="U8" s="61"/>
+      <c r="V8" s="62">
         <v>0</v>
       </c>
-      <c r="W8" s="61">
+      <c r="W8" s="62">
         <v>1</v>
       </c>
-      <c r="X8" s="61">
+      <c r="X8" s="62">
         <v>2</v>
       </c>
-      <c r="Y8" s="61" t="s">
+      <c r="Y8" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="Z8" s="61" t="s">
+      <c r="Z8" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="AA8" s="61" t="s">
+      <c r="AA8" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="AB8" s="61" t="s">
+      <c r="AB8" s="62" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="58"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="66"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="59"/>
       <c r="F9" s="13" t="s">
         <v>53</v>
       </c>
@@ -2695,19 +2731,19 @@
       <c r="O9" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="62"/>
-      <c r="R9" s="62"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
-      <c r="V9" s="61"/>
-      <c r="W9" s="61"/>
-      <c r="X9" s="61"/>
-      <c r="Y9" s="61"/>
-      <c r="Z9" s="61"/>
-      <c r="AA9" s="61"/>
-      <c r="AB9" s="61"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="61"/>
+      <c r="S9" s="61"/>
+      <c r="T9" s="61"/>
+      <c r="U9" s="61"/>
+      <c r="V9" s="62"/>
+      <c r="W9" s="62"/>
+      <c r="X9" s="62"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="62"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="62"/>
     </row>
     <row r="10" spans="2:28" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
@@ -2795,10 +2831,10 @@
       <c r="B12" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="108" t="s">
+      <c r="C12" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="109" t="s">
+      <c r="D12" s="39" t="s">
         <v>100</v>
       </c>
       <c r="E12" s="16" t="s">
@@ -2948,20 +2984,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:O7"/>
-    <mergeCell ref="P7:U7"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="V7:AB7"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N8:O8"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
@@ -2978,6 +3000,20 @@
     <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:O7"/>
+    <mergeCell ref="P7:U7"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="V7:AB7"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2991,8 +3027,8 @@
   </sheetPr>
   <dimension ref="B1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3001,82 +3037,81 @@
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
+    <col min="11" max="12" width="30.6640625" customWidth="1"/>
     <col min="13" max="13" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="84" t="s">
+      <c r="D4" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="75" t="s">
+      <c r="E4" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="75" t="s">
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="76"/>
+      <c r="L4" s="84"/>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="74"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="85"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="107"/>
       <c r="E5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="77" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="78"/>
+      <c r="J5" s="86"/>
       <c r="K5" s="2" t="s">
         <v>62</v>
       </c>
@@ -3088,136 +3123,126 @@
       <c r="B6" s="21">
         <v>9</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="102" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="92" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="93"/>
+      <c r="J6" s="82"/>
       <c r="K6" s="22" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="21">
         <v>10</v>
       </c>
-      <c r="C7" s="79"/>
+      <c r="C7" s="102"/>
       <c r="D7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="21">
-        <v>5</v>
-      </c>
-      <c r="F7" s="21">
-        <v>6</v>
+      <c r="E7" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>111</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="21">
+        <v>1</v>
+      </c>
+      <c r="I7" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="75" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="76"/>
+      <c r="J7" s="84"/>
       <c r="K7" s="21" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
       <c r="L7" s="21" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="21">
         <v>11</v>
       </c>
-      <c r="C8" s="79"/>
+      <c r="C8" s="102"/>
       <c r="D8" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="75" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="76"/>
+      <c r="J8" s="84"/>
       <c r="K8" s="21" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="L8" s="21" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="21">
         <v>12</v>
       </c>
-      <c r="C9" s="79"/>
+      <c r="C9" s="102"/>
       <c r="D9" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="H9" s="21">
+        <v>86400000</v>
+      </c>
+      <c r="I9" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="75" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="76"/>
+      <c r="J9" s="84"/>
       <c r="K9" s="21" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
       <c r="L9" s="21" t="s">
-        <v>20</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>13</v>
       </c>
-      <c r="C10" s="80"/>
-      <c r="D10" s="9" t="s">
-        <v>20</v>
-      </c>
+      <c r="C10" s="103"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="2" t="s">
         <v>20</v>
       </c>
@@ -3230,10 +3255,10 @@
       <c r="H10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="77" t="s">
+      <c r="I10" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="78"/>
+      <c r="J10" s="86"/>
       <c r="K10" s="2" t="s">
         <v>20</v>
       </c>
@@ -3261,129 +3286,141 @@
       <c r="K12" s="23"/>
     </row>
     <row r="13" spans="2:14" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="69" t="s">
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="96" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="70"/>
-      <c r="H13" s="67" t="s">
+      <c r="G13" s="97"/>
+      <c r="H13" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="100" t="s">
+      <c r="I13" s="95"/>
+      <c r="J13" s="95"/>
+      <c r="K13" s="95"/>
+      <c r="L13" s="98"/>
+      <c r="M13" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="N13" s="101"/>
+      <c r="N13" s="93"/>
     </row>
     <row r="14" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="99" t="s">
+      <c r="B14" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="90" t="s">
+      <c r="C14" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="90" t="s">
+      <c r="D14" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="103" t="s">
+      <c r="E14" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="87" t="s">
+      <c r="F14" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="G14" s="86" t="s">
+      <c r="G14" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="H14" s="88" t="s">
+      <c r="H14" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="I14" s="90" t="s">
+      <c r="I14" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="J14" s="90" t="s">
+      <c r="J14" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="K14" s="94" t="s">
+      <c r="K14" s="87" t="s">
         <v>78</v>
       </c>
-      <c r="L14" s="96" t="s">
+      <c r="L14" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="M14" s="98" t="s">
+      <c r="M14" s="91" t="s">
         <v>80</v>
       </c>
-      <c r="N14" s="82" t="s">
+      <c r="N14" s="78" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="102"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="89"/>
-      <c r="I15" s="91"/>
-      <c r="J15" s="91"/>
-      <c r="K15" s="95"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="99"/>
-      <c r="N15" s="87"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="90"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="75"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="27">
-        <f>SUM(C16:D16)</f>
-        <v>0</v>
+      <c r="B16" s="26" t="str">
+        <f>'WBT-TCs'!D8</f>
+        <v>F02_TC03</v>
       </c>
       <c r="C16" s="24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D16" s="24">
         <v>0</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26"/>
+      <c r="E16" s="108">
+        <v>1</v>
+      </c>
+      <c r="F16" s="25"/>
       <c r="G16" s="8" t="s">
         <v>82</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="26">
         <f>SUM(J16:K16)</f>
+        <v>4</v>
+      </c>
+      <c r="J16" s="24">
+        <v>4</v>
+      </c>
+      <c r="K16" s="27">
         <v>0</v>
       </c>
-      <c r="J16" s="24">
-        <v>0</v>
-      </c>
-      <c r="K16" s="28">
-        <v>0</v>
-      </c>
-      <c r="L16" s="29"/>
+      <c r="L16" s="109">
+        <v>1</v>
+      </c>
       <c r="M16" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="N16" s="30">
+      <c r="N16" s="28">
         <f>C16</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="N14:N15"/>
     <mergeCell ref="H14:H15"/>
@@ -3397,19 +3434,11 @@
     <mergeCell ref="L14:L15"/>
     <mergeCell ref="M14:M15"/>
     <mergeCell ref="M13:N13"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3417,15 +3446,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003CE88883EE47F4428D9429E199926803" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f58aede59a59902c28a1e06604e86509">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cb151dce-bb4e-4b45-9888-deda11e2455e" xmlns:ns3="851ad6cb-772e-4066-aadb-684825ca80fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66be19071027bf40cc935f24f7a086f4" ns2:_="" ns3:_="">
     <xsd:import namespace="cb151dce-bb4e-4b45-9888-deda11e2455e"/>
@@ -3614,15 +3634,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD927A50-C247-4539-9D6B-11DFFC9ACCD7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0310686C-5FB0-45DC-A155-16FD14CB70E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3639,4 +3660,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD927A50-C247-4539-9D6B-11DFFC9ACCD7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>